<commit_message>
2019年8月14日00:48:56 new block diagram
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xKang\Desktop\fg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924EC84D-344F-4B1F-8B57-458941F91E3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF72D107-FBF1-49F6-B2B1-38E9E7D81FF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="765" yWindow="1380" windowWidth="28035" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="School" sheetId="4" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>